<commit_message>
Add screws, standoffs, inserts to BOM
</commit_message>
<xml_diff>
--- a/BOM-full.xlsx
+++ b/BOM-full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Fall-2022\Junior-Design\FX-Remote\Whipper-Snapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603AE20B-675B-439E-BF2B-89CC8E0B24AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510EF06B-885F-4403-AC27-6F21E458ED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t xml:space="preserve">Total Price </t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t xml:space="preserve">M2 Heat-Set Knurled Threaded Inserts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M2 Standoffs </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AIEX-Printing-Embedment-Automotive-M2x3x3-5mm/dp/B0B8GN63S2/ref=sr_1_3?keywords=m2+threaded+insert&amp;qid=1667426629&amp;qu=eyJxc2MiOiI0LjUwIiwicXNhIjoiMy44NSIsInFzcCI6IjMuNTYifQ%3D%3D&amp;sprefix=m2+threaded%2Caps%2C147&amp;sr=8-3</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/HELIFOUNER-Spacers-Standoffs-Assortment-Tweezers/dp/B09F8TCLRY/ref=sr_1_4?keywords=m2%2Bstandoffs&amp;qid=1667426997&amp;qu=eyJxc2MiOiIzLjg1IiwicXNhIjoiMy4xNSIsInFzcCI6IjMuMDYifQ%3D%3D&amp;s=industrial&amp;sr=1-4&amp;th=1</t>
   </si>
 </sst>
 </file>
@@ -323,7 +332,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,6 +371,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -644,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1112,6 +1122,17 @@
       <c r="B19" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="G19" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1133,8 +1154,10 @@
     <hyperlink ref="G13" r:id="rId15" xr:uid="{D0D0352E-541D-408D-8485-1D953291E2CB}"/>
     <hyperlink ref="G17" r:id="rId16" xr:uid="{D6F078CB-F670-4BD2-B303-14731B65BDDD}"/>
     <hyperlink ref="G18" r:id="rId17" xr:uid="{E4B0EC92-F11C-41B8-A7EA-68303A4C22B4}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{2CF7B7AE-9793-4AD7-9F67-B97950E2652B}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{C792AC2E-CC5C-40C2-98D7-C9C043EAC52A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add v1 .stl files and imported component models
</commit_message>
<xml_diff>
--- a/BOM-full.xlsx
+++ b/BOM-full.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Fall-2022\Junior-Design\FX-Remote\Whipper-Snapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510EF06B-885F-4403-AC27-6F21E458ED6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C588F0-9605-4257-A71A-DFA88E26B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t xml:space="preserve">Total Price </t>
   </si>
@@ -212,10 +212,16 @@
     <t xml:space="preserve">M2 Standoffs </t>
   </si>
   <si>
-    <t>https://www.amazon.com/AIEX-Printing-Embedment-Automotive-M2x3x3-5mm/dp/B0B8GN63S2/ref=sr_1_3?keywords=m2+threaded+insert&amp;qid=1667426629&amp;qu=eyJxc2MiOiI0LjUwIiwicXNhIjoiMy44NSIsInFzcCI6IjMuNTYifQ%3D%3D&amp;sprefix=m2+threaded%2Caps%2C147&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/HELIFOUNER-Spacers-Standoffs-Assortment-Tweezers/dp/B09F8TCLRY/ref=sr_1_4?keywords=m2%2Bstandoffs&amp;qid=1667426997&amp;qu=eyJxc2MiOiIzLjg1IiwicXNhIjoiMy4xNSIsInFzcCI6IjMuMDYifQ%3D%3D&amp;s=industrial&amp;sr=1-4&amp;th=1</t>
+    <t>https://www.amazon.com/HELIFOUNER-Spacers-Standoffs-Assortment-Tweezers/dp/B09F8TCLRY/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/AIEX-Printing-Embedment-Automotive-M2x3x3-5mm/dp/B0B8GN63S2/</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2178</t>
+  </si>
+  <si>
+    <t>5mm Chromed Wide Concave Bevel LED Holder</t>
   </si>
 </sst>
 </file>
@@ -332,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,6 +378,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -654,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1123,7 +1132,7 @@
         <v>56</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
@@ -1131,7 +1140,27 @@
         <v>57</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2178</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1156,8 +1185,9 @@
     <hyperlink ref="G18" r:id="rId17" xr:uid="{E4B0EC92-F11C-41B8-A7EA-68303A4C22B4}"/>
     <hyperlink ref="G19" r:id="rId18" xr:uid="{2CF7B7AE-9793-4AD7-9F67-B97950E2652B}"/>
     <hyperlink ref="G20" r:id="rId19" xr:uid="{C792AC2E-CC5C-40C2-98D7-C9C043EAC52A}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{10A5A26B-B636-44B3-96F4-6329C64E7632}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update base .stl file, add media
</commit_message>
<xml_diff>
--- a/BOM-full.xlsx
+++ b/BOM-full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\Fall-2022\Junior-Design\FX-Remote\Whipper-Snapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C588F0-9605-4257-A71A-DFA88E26B021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE90F2E-7CB2-4FEB-B838-8A51BEBB239D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t xml:space="preserve">Total Price </t>
   </si>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1131,6 +1131,15 @@
       <c r="B19" s="7" t="s">
         <v>56</v>
       </c>
+      <c r="C19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
       <c r="G19" s="14" t="s">
         <v>59</v>
       </c>
@@ -1138,6 +1147,15 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>57</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>58</v>

</xml_diff>